<commit_message>
Criado notebooks para primeira aula
</commit_message>
<xml_diff>
--- a/ementa/DS&AI - Feature Engineering - Ementa.xlsx
+++ b/ementa/DS&AI - Feature Engineering - Ementa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\GitHub\FIAP-Feature-Engineering\ementa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D8483D-C757-4778-B805-02B64D07497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A47691F-7646-4BD8-8DDA-17D9E784164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="6708" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ementa" sheetId="1" r:id="rId1"/>
@@ -466,39 +466,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -845,7 +845,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,28 +859,28 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -967,7 +967,7 @@
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="13"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
@@ -992,7 +992,7 @@
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
@@ -1017,12 +1017,12 @@
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
@@ -1075,7 +1075,7 @@
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
@@ -1084,54 +1084,49 @@
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A35:C35"/>
@@ -1146,6 +1141,11 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C6:C10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C24" r:id="rId1" display="https://www.anaconda.com/download/" xr:uid="{4CB0E2AC-91DD-480B-B5ED-C96D8B39C866}"/>
@@ -1165,15 +1165,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100968740B4C0987B4D86879E800A26E446" ma:contentTypeVersion="6" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="40148e4f47cd1cf31e6bb17e81f72657">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2220af93-035a-443f-80b0-3b9b401ad9a6" xmlns:ns3="d48fd270-4a57-47e1-b674-c7d4969804ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f6914669f2d55499eb4d18a71643d5e2" ns2:_="" ns3:_="">
     <xsd:import namespace="2220af93-035a-443f-80b0-3b9b401ad9a6"/>
@@ -1350,6 +1341,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0676F046-680E-4D82-9A09-EAE9415B8415}">
   <ds:schemaRefs>
@@ -1360,14 +1360,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DD008-02E9-4597-9992-2733F6487F15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D6FA30-3055-41DE-801B-394F36D06871}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1384,4 +1376,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DD008-02E9-4597-9992-2733F6487F15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adicionado notebooks da aula 2 e melhorados notebooks da aula 1.
</commit_message>
<xml_diff>
--- a/ementa/DS&AI - Feature Engineering - Ementa.xlsx
+++ b/ementa/DS&AI - Feature Engineering - Ementa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\GitHub\FIAP-Feature-Engineering\ementa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A47691F-7646-4BD8-8DDA-17D9E784164A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8960E11-35C9-4154-9D15-EB3956922ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="6708" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,48 +466,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,28 +859,28 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="10"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -967,7 +967,7 @@
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
@@ -992,10 +992,10 @@
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="21">
+      <c r="A18" s="19">
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1006,23 +1006,23 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="23"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
@@ -1075,7 +1075,7 @@
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="15"/>
+      <c r="A28" s="13"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
@@ -1084,49 +1084,54 @@
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C6:C10"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A35:C35"/>
@@ -1141,11 +1146,6 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="C18:C20"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C24" r:id="rId1" display="https://www.anaconda.com/download/" xr:uid="{4CB0E2AC-91DD-480B-B5ED-C96D8B39C866}"/>
@@ -1165,6 +1165,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100968740B4C0987B4D86879E800A26E446" ma:contentTypeVersion="6" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="40148e4f47cd1cf31e6bb17e81f72657">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2220af93-035a-443f-80b0-3b9b401ad9a6" xmlns:ns3="d48fd270-4a57-47e1-b674-c7d4969804ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f6914669f2d55499eb4d18a71643d5e2" ns2:_="" ns3:_="">
     <xsd:import namespace="2220af93-035a-443f-80b0-3b9b401ad9a6"/>
@@ -1341,15 +1350,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0676F046-680E-4D82-9A09-EAE9415B8415}">
   <ds:schemaRefs>
@@ -1360,6 +1360,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DD008-02E9-4597-9992-2733F6487F15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D6FA30-3055-41DE-801B-394F36D06871}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1376,12 +1384,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DD008-02E9-4597-9992-2733F6487F15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adicionado exercício para aula 1 e notebook para transformação de dados não estruturados
</commit_message>
<xml_diff>
--- a/ementa/DS&AI - Feature Engineering - Ementa.xlsx
+++ b/ementa/DS&AI - Feature Engineering - Ementa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\GitHub\FIAP-Feature-Engineering\ementa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8960E11-35C9-4154-9D15-EB3956922ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC247C8-5D7F-49E7-8E9C-CB289AEE02FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6708" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ementa" sheetId="1" r:id="rId1"/>
@@ -466,48 +466,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -844,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,28 +859,28 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -967,7 +967,7 @@
       <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="13"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11">
@@ -992,10 +992,10 @@
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="19">
+      <c r="A18" s="21">
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1006,23 +1006,23 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
@@ -1075,7 +1075,7 @@
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="13"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
@@ -1084,54 +1084,49 @@
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C6:C10"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A35:C35"/>
@@ -1146,6 +1141,11 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C6:C10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C24" r:id="rId1" display="https://www.anaconda.com/download/" xr:uid="{4CB0E2AC-91DD-480B-B5ED-C96D8B39C866}"/>
@@ -1165,15 +1165,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100968740B4C0987B4D86879E800A26E446" ma:contentTypeVersion="6" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="40148e4f47cd1cf31e6bb17e81f72657">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2220af93-035a-443f-80b0-3b9b401ad9a6" xmlns:ns3="d48fd270-4a57-47e1-b674-c7d4969804ad" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f6914669f2d55499eb4d18a71643d5e2" ns2:_="" ns3:_="">
     <xsd:import namespace="2220af93-035a-443f-80b0-3b9b401ad9a6"/>
@@ -1350,6 +1341,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0676F046-680E-4D82-9A09-EAE9415B8415}">
   <ds:schemaRefs>
@@ -1360,14 +1360,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DD008-02E9-4597-9992-2733F6487F15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D6FA30-3055-41DE-801B-394F36D06871}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1384,4 +1376,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF5DD008-02E9-4597-9992-2733F6487F15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>